<commit_message>
Events sepeated in different  columns
</commit_message>
<xml_diff>
--- a/club.xlsx
+++ b/club.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motat\OneDrive\Desktop\CSPIT_NEW_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BD219D-C060-47CC-92F0-62B3A865E8B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60005286-5E91-4987-88E0-F07AB888D74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="120">
   <si>
     <t>Club ID</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Student Coordinators</t>
   </si>
   <si>
-    <t>Events</t>
-  </si>
-  <si>
     <t>AWS Student Club</t>
   </si>
   <si>
@@ -377,6 +374,18 @@
   </si>
   <si>
     <t>images1\Student Club\ML_Club.webp</t>
+  </si>
+  <si>
+    <t>Event 1</t>
+  </si>
+  <si>
+    <t>AWS Cloud Bootcamp, A three-day coding event, 15-17 Nov 2023, images1/gallery/AWS Commuinity Day/aws2.webp:images1/gallery/AWS Commuinity Day/aws1.webp:images1/gallery/AWS Commuinity Day/aws3.webp:images1/gallery/AWS Commuinity Day/aws5.webp</t>
+  </si>
+  <si>
+    <t>AWS Community Day, A three-day coding event, 15-17 Nov 2023,   images1/gallery/AWS Commuinity Day/aws2.webp:images1/gallery/AWS Commuinity Day/aws1.webp:images1/gallery/AWS Commuinity Day/aws3.webp:images1/gallery/AWS Commuinity Day/aws5.webp</t>
+  </si>
+  <si>
+    <t>Event 2</t>
   </si>
 </sst>
 </file>
@@ -733,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:G44"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -748,9 +757,10 @@
     <col min="5" max="5" width="40.77734375" customWidth="1"/>
     <col min="6" max="6" width="29.21875" customWidth="1"/>
     <col min="7" max="7" width="47.44140625" customWidth="1"/>
+    <col min="8" max="8" width="31.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -770,258 +780,264 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>21</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>25</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="D7" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>37</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="C9" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>86</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1062,389 +1078,389 @@
   <sheetData>
     <row r="1" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="D2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="D3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>59</v>
-      </c>
       <c r="H3" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>26</v>
-      </c>
       <c r="E4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>62</v>
-      </c>
       <c r="H4" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="E5" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>65</v>
-      </c>
       <c r="H5" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="E6" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="H6" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="E7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>71</v>
-      </c>
       <c r="H7" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="E8" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>74</v>
-      </c>
       <c r="H8" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="D9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="H9" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>83</v>
-      </c>
       <c r="H10" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>89</v>
-      </c>
       <c r="H11" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>94</v>
-      </c>
       <c r="H12" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>101</v>
-      </c>
       <c r="H13" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="G14" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>108</v>
-      </c>
       <c r="H14" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="F15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>113</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Club sheet data update
</commit_message>
<xml_diff>
--- a/club.xlsx
+++ b/club.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motat\OneDrive\Desktop\CSPIT_NEW_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\CSPIT_Main\CSPIT_NEW_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF0C4A6-F231-4BDA-9D8F-1AEF90275479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB7CD09-CB62-40C2-A613-B48FC6B8C556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="185">
   <si>
     <t>Club ID</t>
   </si>
@@ -61,12 +61,6 @@
     <t xml:space="preserve">Dulari Bhushan; Parmesh Bhatt </t>
   </si>
   <si>
-    <t>CSPIT_Faculty\IT\SANKETKUMAR.webp</t>
-  </si>
-  <si>
-    <t>CSPIT_Faculty\IT\PARTH.webp</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Dr. Parth Shah,faculty cordinator,parthshah.it@charusat.ac.in,99999,CSPIT_Faculty\IT\PARTH.webp;Dr. Sanket Suthar,faculty cordinator,sanketsuthar.it@charusat.ac.in,999999,CSPIT_Faculty\IT\SANKETKUMAR.webp</t>
   </si>
   <si>
@@ -389,13 +383,290 @@
   </si>
   <si>
     <t>Gallery</t>
+  </si>
+  <si>
+    <t>The AI/ML Club of the CSE Department is a vibrant community dedicated to exploring the vast potential of Artificial Intelligence and Machine Learning. Our mission is to bridge the gap between theory and real-world applications through workshops, expert talks, hands-on projects, hackathons, and research initiatives. Whether you're a beginner or an experienced enthusiast, the club provides opportunities to learn, collaborate, and innovate in cutting-edge AI technologies. By fostering creativity and technical expertise, we aim to shape the future of AI and empower students to make a meaningful impact in the digital world.</t>
+  </si>
+  <si>
+    <t>Tribe of Creativity aims to organize cultural and sports activities while providing a platform for students to showcase their creativity and teamwork. The club fosters sportsmanship, leadership, confidence, and collaboration through engaging events, encouraging holistic development beyond academics.</t>
+  </si>
+  <si>
+    <t>Club Gamma is a student-driven tech community focused on open-source development, innovation, and collaborative learning. It provides a platform for students to enhance their coding skills, work on real-world projects, and participate in hackathons. The club fosters a culture of knowledge sharing, mentorship, and teamwork, helping members grow in various domains of technology.</t>
+  </si>
+  <si>
+    <t>The Cyber Security Club is a peer-learning community where students collaborate to explore various aspects of cybersecurity. It provides a platform for members to share knowledge, discuss emerging threats, and work on real-world security challenges. Through workshops, hands-on sessions, and group discussions, participants enhance their technical skills and stay updated with industry trends. The club fosters a learning environment that encourages problem-solving, ethical hacking, and secure coding practices. Whether beginners or advanced learners, all members contribute to and benefit from the collective expertise of the group.</t>
+  </si>
+  <si>
+    <t>Data science is a multidisciplinary approach to extracting actionable insights from the large and ever-increasing volumes of data collected and created by today’s organizations. Data science encompasses preparing data for analysis and processing, performing advanced data analysis, and presenting the results to reveal patterns and enable stakeholders to draw informed conclusions. The Data Science Club’s primary objective is to unify colleges across the country that want to promote Data Science as a desirable career path to their students by getting them to join our revolutionary career-oriented corporate club.</t>
+  </si>
+  <si>
+    <t>The Machine Learning (ML) Club at the U &amp; P U. Patel Department of Computer Engineering, CSPIT, provides a platform for students to explore and apply Machine Learning, Deep Learning, and AI techniques. The club fosters learning through workshops, hands-on sessions, research discussions, and real-world projects. It encourages collaboration, innovation, and problem-solving through hackathons, competitions, and industry interactions. The club aims to bridge the gap between theoretical concepts and practical applications, helping students gain expertise in tools like Python, TensorFlow, and PyTorch. The first session will focus on Applications of ML, DL, and Generative AI, inspiring students to explore cutting-edge advancements.</t>
+  </si>
+  <si>
+    <t>House of Innovation - Skills for Life is the club which has been established by the mechanical engineering students. The aim to establish this club is to provide the  technical &amp; non-technical skills as well as knowledge. Here, the method we follow is “best way to learn is to teach others” under the guidance of specilist provided by the mechanical department, charusat. 
+This club conducts seminars, sessions for life skills, soft skills and also classes for language learning.</t>
+  </si>
+  <si>
+    <t>The VLSI Club is a dynamic platform dedicated to fostering innovation and skill development in the semiconductor ecosystem. Its objective is to bridge the industry-academia gap by organizing expert talks, summits, and industry connect series, enabling students to engage with professionals and emerging technologies. The club hosts hackathons, peer-to-peer learning sessions, and hands-on projects, encouraging practical exposure to VLSI design and verification. Through project demonstrations and activity-based learning, members gain real-world experience in chip design, fabrication, and testing. Additionally, the club facilitates mentorship programs, research collaborations, and startup incubation support, empowering the next generation of semiconductor professionals.</t>
+  </si>
+  <si>
+    <t>The Competitive Programming Squad is a community of passionate coders dedicated to mastering problem-solving and algorithmic skills. The club fosters innovation, collaboration, and excellence, preparing members for national and international coding competitions. Through regular practice, coding contests, and peer learning, it aims to build a strong coding culture and equip students with the expertise to thrive in the competitive programming landscape.</t>
+  </si>
+  <si>
+    <t>The Eloquence Club  is dedicated to fostering a vibrant community of individuals equipped with essential soft skills, empowering them to excel in both their personal and professional lives. With a strong commitment to continuous learning, practice, and growth, the club serves as a platform where students can refine their communication, teamwork, leadership, and adaptability—skills that are crucial for success in today's dynamic world.  
+Through a variety of engaging events and activities, the Eloquence Club provides opportunities for students to develop confidence, articulate their thoughts effectively, and collaborate seamlessly. Our mission is to nurture individuals who are not only competent in their respective fields but also capable of making a meaningful impact through their enhanced interpersonal abilities.</t>
+  </si>
+  <si>
+    <t>The Debate Club at the M. S. Patel Department of Civil Engineering is a dynamic platform for fostering critical thinking, effective communication, and collaborative learning among students. Our club aims to ignite intellectual curiosity and promote the art of structured argumentation, which is an essential skill for future engineers. Through regular sessions, members engage in thought- provoking debates on a variety of topics, ranging from current affairs and societal issues to technical advancements in civil engineering. These debates encourage students to explore diverse perspectives, hone their research skills, and present their ideas persuasively.
+The club provides a supportive and inclusive environment where participants can build confidence in public speaking and develop teamwork and leadership abilities. Experienced faculty mentors and guest speakers often guide sessions, offering valuable insights and feedback to enhance the learning experience.
+In addition to in-house activities, the Debate Club actively participates in intercollegiate competitions, showcasing the talent and preparedness of our students on larger platforms. These events not only bring recognition to the department but also foster camaraderie and a spirit of healthy competition among peers.
+The Debate Club is more than just a forum for discussion; it’s a community that nurtures analytical minds and empowers students to become articulate professionals ready to tackle the challenges of the modern world.</t>
+  </si>
+  <si>
+    <t>A Code for Cause club is a coding club where a 
+group ofinterested and enthusiastic students who
+ learn and practicecoding together in a 
+supportive environment. The Code forCause
+ club develops programming skills, computational
+ skills andlogical skills. In this club activities, 
+students can enhance their knowledge and
+ experience how to convert the knowledge in real
+time applications. This club provides a platform
+ for the students to embedded certain hardware
+ tools and particular code. The students are 
+encouraged to participate in various technical 
+competitions such as hackathon, codefiesta etc.</t>
+  </si>
+  <si>
+    <t>Apurv Chudasama;
+Krushna Parmar</t>
+  </si>
+  <si>
+    <t>Kaushal; Pooja</t>
+  </si>
+  <si>
+    <t>Jalay Movaliya;
+Jay Khatri;
+Pooja Ramani;
+Mit Monpara; 
+Bhavya Prajapati;
+Jay Rupapara;
+Charmi Dodiya; 
+Satyam Charola;
+Dhairya Kanabar; 
+Dhiraj Bagad;
+Kaushal Bhanderi;
+Shrey Lakhtaria</t>
+  </si>
+  <si>
+    <t>Darshil Chocha; Yupal Chaudhari</t>
+  </si>
+  <si>
+    <t>Rinkal Mav</t>
+  </si>
+  <si>
+    <t>Jash Bhungalia;
+Shradhha Lal</t>
+  </si>
+  <si>
+    <t>Dev Parikh;
+Yashvi Thakkar</t>
+  </si>
+  <si>
+    <t>Dhruti Panchal</t>
+  </si>
+  <si>
+    <t>Nilay Shah;
+Nishit Patel</t>
+  </si>
+  <si>
+    <t>Anurag Ladumor;
+Aastha Soni;
+Pearl Patel;
+Dhyey Amin</t>
+  </si>
+  <si>
+    <t>Harsh Desai</t>
+  </si>
+  <si>
+    <t>Vedansh Verdia</t>
+  </si>
+  <si>
+    <t>AI for All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI for All Club is an inclusive community where students from diverse backgrounds come together to explore the fascinating world of artificial intelligence. The club aims to build foundational and advanced AI knowledge by covering key topics such as machine learning, deep learning, natural language processing, and computer vision.Through hands-on projects, workshops, and discussions, students gain practical experience in applying AI to real-world problems. </t>
+  </si>
+  <si>
+    <t>Kachiyapatel Mahi</t>
+  </si>
+  <si>
+    <t>CyberKavach Club</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyber Kavach is student-oriented community that is committed to fostering hands-on peer learning sessions, knowledge-sharing, and collaboration to tackle emerging cyber challenges. Through practical hands-on experience and Industry exposure, the club aims to equip its members with the tools and expertise to defend the digital cyber world.
+</t>
+  </si>
+  <si>
+    <t>Prince Tadhani</t>
+  </si>
+  <si>
+    <t>EyeCoders</t>
+  </si>
+  <si>
+    <t>The Eye Coders Club, brought to you by the Department of Computer Science &amp; Engineering at CSPIT, CHARUSAT, is more than just a club. 
+it's an opportunity to dive into the world of Competitive Programming and reap its many benefits. 
+Our goal is to inspire and prepare our student community for the challenges ahead.</t>
+  </si>
+  <si>
+    <t>Darsh Patel; Jayraj Lakkad</t>
+  </si>
+  <si>
+    <t>Grow With Git</t>
+  </si>
+  <si>
+    <t>Provide a platform for students to learn and master version control using Git and GitHub.
+Foster collaboration and knowledge-sharing among students interested in software development.
+Organize workshops, seminars, and coding competitions to enhance students skills in using Git and
+GitHub.
+Encourage students to contribute to open-source projects and build a strong portfolio.
+Facilitate networking opportunities with industry professionals and alumni through guest lectures
+and events.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Darsh Patel; Shail Macwan; Piyanshu Chanaria</t>
+  </si>
+  <si>
+    <t>Innovators Club: Prepare, Compete, Grow</t>
+  </si>
+  <si>
+    <t>The Innovators Club is a dynamic platform for students who are passionate about creativity, technology, and problem-solving. To empower students to develop cutting-edge projects, compete in prestigious events,and cultivate professional networks that will propel their careers.This club fosters innovation by encouraging students to explore emerging technologies, brainstorm new ideas, and develop solutions for real-world challenges.Through hands-on projects, workshops, and interdisciplinary collaboration, members can enhance their critical thinking, design thinking, and prototyping skills.</t>
+  </si>
+  <si>
+    <t>Math for AI</t>
+  </si>
+  <si>
+    <t>Robotics Club (Institute Level)</t>
+  </si>
+  <si>
+    <t>Math for AI Club is a dedicated community where passionate and curious students come together to explore the mathematical foundations of artificial intelligence. The club focuses on developing strong mathematical skills, including linear algebra, probability, statistics, and calculus, which are essential for understanding and building AI models. Through various activities, students can deepen their knowledge and experience how mathematical concepts are applied in real-world AI applications. This club provides a platform for students to experiment with mathematical modeling, optimization techniques, and AI-related problem-solving.</t>
+  </si>
+  <si>
+    <t>Robotics Club aims to provide a platform for enthusiasts like yourself to come 
+together, learn, innovate, and explore the fascinating world of robotics. 
+Whether you're a seasoned enthusiast or just curious about this rapidly advancing field, there's a place for you in our club.</t>
+  </si>
+  <si>
+    <t>Rohan Vaghela;
+Pruthvish Dave</t>
+  </si>
+  <si>
+    <t>SpiriTech Club</t>
+  </si>
+  <si>
+    <t>Prof. Harshul Yagnik,faculty coordinator,harshulyagnik.cse@charusat.ac.in,9737642757,CSPIT_Faculty\CSE\HARSHULYAGNIK.webp;Prof. Abhishek Patel,faculty coordinator,abhishekpatel.cse@charusat.ac.in,9099056918,CSPIT_Faculty\CSE\ABHISHEKPATEL.webp</t>
+  </si>
+  <si>
+    <t>Prof. Trusha Patel,faculty coordinator,trushagajjar.ce@charusat.ac.in,9624699433,CSPIT_Faculty\CE\TRUSHAPATEL.webp;Prof. Rikita Chokshi,faculty coordinator,rikitachokshi.ce@charusat.ac.in,8780797085,CSPIT_Faculty\CE\RIKITACHOKSHI.webp</t>
+  </si>
+  <si>
+    <t>Dr. Mrugendra Rahevar,faculty coordinator,mrugendrarahevar.ce@charusat.ac.in,9925856399,CSPIT_Faculty\CE\MRUGENDRARAHEVAR.webp;
+Prof. Ronak R Patel,faculty coordinator,ronakrpatel.ce@charusat.ac.in,9409330900,CSPIT_Faculty\CE\RONAKRPATEL.webp;
+Prof. Trusha Patel,faculty coordinator,trushagajjar.ce@charusat.ac.in,9624699443,CSPIT_Faculty\CE\TRUSHAPATEL.webp;
+Prof. Vaishali Koria,faculty coordinator,vaishalimewada.ce@charusat.ac.in,7874114875,CSPIT_Faculty\CE\VAISHALIKORIA.webp</t>
+  </si>
+  <si>
+    <t>Dr. Martin Parmar,faculty coordinator,martinparmar.ce@charusat.ac.in,8238563982,CSPIT_Faculty\CE\MARTINPARMAR.webp;
+Dr. Sneha Padhiar,faculty coordinator,snehapadhiar.ce@charusat.ac.in,9601600000,CSPIT_Faculty\CE\SNEHAPADHIAR.webp</t>
+  </si>
+  <si>
+    <t>Jalpesh Vasa,faculty coordinator,jalpeshvasa.it@charusat.ac.in,9726528769,CSPIT_Faculty\IT\JALPESHVASA.webp;
+Hemant Yadav,faculty coordinator,hemantyadav.it@charusat.ac.in,9327083391,CSPIT_Faculty\IT\HEMANTYADAV.webp</t>
+  </si>
+  <si>
+    <t>Dr. Mrugendra Rahevar,faculty coordinator,mrugendrarahevar.ce@charusat.ac.in,9925856399,CSPIT_Faculty\CE\MRUGENDRARAHEVAR.webp;
+Prof. Ronak N Patel,faculty coordinator,ronakpatel.ce@charusat.ac.in,9913760408,CSPIT_Faculty\CE\RONAKNPATEL.webp;
+Dr. Dhaval Bhoi,faculty coordinator,dhavalbhoi.ce@charusat.ac.in,9879974807,CSPIT_Faculty\CE\DHAVALBHOI.webp</t>
+  </si>
+  <si>
+    <t>Prof. Vikas Panchal,faculty coordinator,vikaspanchal.me@charusat.ac.in,8866286233,CSPIT_Faculty\ME\VIKASPANCHAL.webp;</t>
+  </si>
+  <si>
+    <t>Dr. Arpita Patel,faculty coordinator,N/A,9428661555,CSPIT_Faculty\N/A\ARPITAPATEL.webp</t>
+  </si>
+  <si>
+    <t>Prof. Nishat Shaikh,faculty coordinator,nishatshaikh.it@charusat.ac.in,9979157363,CSPIT_Faculty\IT\NISHATSHAIKH.webp</t>
+  </si>
+  <si>
+    <t>Prof. Nishat Shaikh,faculty coordinator,nishatshaikh.it@charusat.ac.in,9979157363,CSPIT_Faculty\IT\NISHATSHAIKH.webp;
+Dr. Parth Shah,faculty coordinator,parthshah.ce@charusat.ac.in,9925020358,CSPIT_Faculty\CE\PARTHSHAH.webp</t>
+  </si>
+  <si>
+    <t>Prof. Pinal Patel,faculty coordinator,N/A,9979975075,CSPIT_Faculty\N/A\PINALPATEL.webp;
+Prof. Megha Desai,faculty coordinator,N/A,9429032853,CSPIT_Faculty\N/A\MEGHADESAI.webp;
+Prof. Neha Rajput,faculty coordinator,N/A,9099027974,CSPIT_Faculty\N/A\NEHARAJPUT.webp;
+Prof. Gargi Ray,faculty coordinator,N/A,8238042155,CSPIT_Faculty\N/A\GARGIRAY.webp</t>
+  </si>
+  <si>
+    <t>Prof. Kanchal Dave,faculty coordinator,N/A,9973054924,CSPIT_Faculty\N/A\KANCHALDAVE.webp;
+Prof. Mehul Katakiya,faculty coordinator,N/A,8000669363,CSPIT_Faculty\N/A\MEHULKATAKIYA.webp;
+Prof. Vipul Vyas,faculty coordinator,N/A,9727767541,CSPIT_Faculty\N/A\VIPULVYAS.webp;
+Prof. Jay Bhavsar,faculty coordinator,N/A,9898583301,CSPIT_Faculty\N/A\JAYBHAVSAR.webp</t>
+  </si>
+  <si>
+    <t>Dr. Killol Pandya,faculty coordinator,N/A,7600004093,CSPIT_Faculty\N/A\KILLOLPANDYA.webp</t>
+  </si>
+  <si>
+    <t>Dr. Nirav Bhatt,faculty coordinator,niravbhatt.it@charusat.ac.in,9998582812,CSPIT_Faculty\IT\NIRAVBHATT.webp</t>
+  </si>
+  <si>
+    <t>Prof. Dharmendrasinh Rathod,faculty coordinator,dharmendrarathod.cse@charusat.ac.in,9510406252,CSPIT_Faculty\CSE\DHARMENDRASINHRATHOD.webp;
+Prof. Hemang Thakar,faculty coordinator,hemangthakar.cse@charusat.ac.in,9409404004,CSPIT_Faculty\CSE\HEMANGTHAKAR.webp</t>
+  </si>
+  <si>
+    <t>Prof. Dhara Solanki,faculty coordinator,dharasolanki.cse@charusat.ac.in,8238448451,CSPIT_Faculty\CSE\DHARASOLANKI.webp;
+Prof. Srushti Gajjar,faculty coordinator,srushtigajjar.cse@charusat.ac.in,9409546741,CSPIT_Faculty\CSE\SRUSHTIGAJJAR.webp;
+Prof. Brinda Patel,faculty coordinator,brindapatel.cse@charusat.ac.in,7405281125,CSPIT_Faculty\CSE\BRINDAPATEL.webp</t>
+  </si>
+  <si>
+    <t>Prof. Jalpa Ardeshana,faculty coordinator,jalpaardeshana.aiml@charusat.ac.in,6354272052,CSPIT_Faculty\AIML\JALPAARDESHANA.webp</t>
+  </si>
+  <si>
+    <t>Dr. Spoorthy V,faculty coordinator,spoorthy.aiml@charusat.ac.in,8310726037,CSPIT_Faculty\AIML\SPOORTHYV.webp</t>
+  </si>
+  <si>
+    <t>Dr. Upesh Patel,faculty coordinator,N/A,9913759877,CSPIT_Faculty\N/A\UPESHPATEL.webp;
+Dr. Jigar Sarda,faculty coordinator,N/A,N/A,CSPIT_Faculty\N/A\JIGARSARDA.webp;
+Dr. Dipal Patel,faculty coordinator,N/A,N/A,CSPIT_Faculty\N/A\DIPALPATEL.webp;
+Dr. Miral Desai,faculty coordinator,N/A,N/A,CSPIT_Faculty\N/A\MIRALDESAI.webp</t>
+  </si>
+  <si>
+    <t>Prof. Vaibhavi Patel,faculty coordinator,vaibhavipatel.cse@charusat.ac.in,6359357364,CSPIT_Faculty\CSE\VAIBHAVIPATEL.webp;
+Prof. Avani Khokhariya,faculty coordinator,N/A,N/A,CSPIT_Faculty\CSE\AVANIKHOKHARIYA.webp</t>
+  </si>
+  <si>
+    <t>Kesha Desai; Pooja Mehta;
+Pooja Rachchh;
+Anshu Trivedi;
+Manan Panchal;
+Krish Singh</t>
+  </si>
+  <si>
+    <t>Aum Barai;
+Saumya Gohil;
+Krushna Parmar;
+Twisha Kamani;
+Sanskruti Kukadiya;
+Yug Bhatt;
+Hitarth Khatiwala</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,6 +690,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -428,7 +710,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -436,12 +718,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -469,6 +766,19 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -751,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="66" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,13 +1100,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K1" s="1"/>
     </row>
@@ -808,279 +1118,455 @@
         <v>6</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K3" s="9"/>
     </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+        <v>119</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4" s="5"/>
       <c r="H4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="B7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="B8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>37</v>
-      </c>
       <c r="B9" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="3"/>
+        <v>124</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+        <v>125</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>136</v>
+      </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>78</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+        <v>126</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="D13" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>172</v>
+      </c>
       <c r="F13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D15" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>109</v>
+      <c r="D16" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16" t="s">
+        <v>175</v>
+      </c>
+      <c r="F16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="179.4" x14ac:dyDescent="0.3">
+      <c r="B17" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="202.8" x14ac:dyDescent="0.3">
+      <c r="B18" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="B19" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="248.4" x14ac:dyDescent="0.3">
+      <c r="B21" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="248.4" x14ac:dyDescent="0.3">
+      <c r="B22" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="B23" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="156" x14ac:dyDescent="0.3">
+      <c r="B24" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="F24" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H4" r:id="rId1" xr:uid="{B3799252-325C-4BA7-83E1-0B4ABA4630D6}"/>
-    <hyperlink ref="E8" r:id="rId2" xr:uid="{B861C936-E4F5-4280-A1E9-D2DB6589BA9A}"/>
-    <hyperlink ref="E9" r:id="rId3" xr:uid="{E4999B8B-293D-4990-A766-84FC6D5195B5}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{C053D9B7-E09A-4F85-9B15-3356C9467DDC}"/>
-    <hyperlink ref="C3" r:id="rId5" xr:uid="{A130776E-467C-4CF5-A279-81C121EAFA77}"/>
-    <hyperlink ref="C9" r:id="rId6" xr:uid="{C43E63E5-175D-482B-8E60-565A2317DAF1}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{2EB0C192-8899-4B0D-BC90-80D1B99B5AD3}"/>
-    <hyperlink ref="C7" r:id="rId8" xr:uid="{C7E09B01-0EAD-4328-8C47-DBFCB5792DCE}"/>
-    <hyperlink ref="C4" r:id="rId9" xr:uid="{2F6D441B-FE18-407A-A53C-332DADE184B6}"/>
-    <hyperlink ref="C5" r:id="rId10" xr:uid="{D9ABECE2-61DA-4365-A359-C85CF5D16BC9}"/>
-    <hyperlink ref="C6" r:id="rId11" xr:uid="{C9477454-ED77-4337-AC39-DDF8661E5749}"/>
-    <hyperlink ref="C10" r:id="rId12" xr:uid="{C71A858D-5AD9-4C78-8958-2F44E3B2D91B}"/>
-    <hyperlink ref="C11" r:id="rId13" xr:uid="{FA9B5FF1-66E1-4867-BB96-B75C16AF9696}"/>
-    <hyperlink ref="C12" r:id="rId14" xr:uid="{B5F89BDF-DA28-43E9-BC34-ABA3C0433BB1}"/>
-    <hyperlink ref="C13" r:id="rId15" xr:uid="{384BE91D-6FD8-446A-BAA4-C63875390E3C}"/>
-    <hyperlink ref="C14" r:id="rId16" xr:uid="{5F462241-14AD-4645-BE81-22C387C87ACC}"/>
-    <hyperlink ref="C15" r:id="rId17" xr:uid="{25B1CA69-2415-4C8C-AEF6-44FD92D413C8}"/>
-    <hyperlink ref="C16" r:id="rId18" xr:uid="{18DAC898-53DE-4C70-BD52-48C6FF1513F1}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{C053D9B7-E09A-4F85-9B15-3356C9467DDC}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{A130776E-467C-4CF5-A279-81C121EAFA77}"/>
+    <hyperlink ref="C9" r:id="rId4" xr:uid="{C43E63E5-175D-482B-8E60-565A2317DAF1}"/>
+    <hyperlink ref="C8" r:id="rId5" xr:uid="{2EB0C192-8899-4B0D-BC90-80D1B99B5AD3}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{C7E09B01-0EAD-4328-8C47-DBFCB5792DCE}"/>
+    <hyperlink ref="C4" r:id="rId7" xr:uid="{2F6D441B-FE18-407A-A53C-332DADE184B6}"/>
+    <hyperlink ref="C5" r:id="rId8" xr:uid="{D9ABECE2-61DA-4365-A359-C85CF5D16BC9}"/>
+    <hyperlink ref="C6" r:id="rId9" xr:uid="{C9477454-ED77-4337-AC39-DDF8661E5749}"/>
+    <hyperlink ref="C10" r:id="rId10" xr:uid="{C71A858D-5AD9-4C78-8958-2F44E3B2D91B}"/>
+    <hyperlink ref="C11" r:id="rId11" xr:uid="{FA9B5FF1-66E1-4867-BB96-B75C16AF9696}"/>
+    <hyperlink ref="C12" r:id="rId12" xr:uid="{B5F89BDF-DA28-43E9-BC34-ABA3C0433BB1}"/>
+    <hyperlink ref="C13" r:id="rId13" xr:uid="{384BE91D-6FD8-446A-BAA4-C63875390E3C}"/>
+    <hyperlink ref="C14" r:id="rId14" xr:uid="{5F462241-14AD-4645-BE81-22C387C87ACC}"/>
+    <hyperlink ref="C15" r:id="rId15" xr:uid="{25B1CA69-2415-4C8C-AEF6-44FD92D413C8}"/>
+    <hyperlink ref="C16" r:id="rId16" xr:uid="{18DAC898-53DE-4C70-BD52-48C6FF1513F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 
@@ -1102,383 +1588,383 @@
         <v>6</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="E2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="E3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>57</v>
-      </c>
       <c r="H3" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="E4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="H4" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="E5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="H5" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>32</v>
-      </c>
       <c r="E6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="H6" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="E7" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="H7" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="E8" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>72</v>
-      </c>
       <c r="H8" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="E9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>75</v>
-      </c>
       <c r="H9" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="F10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>81</v>
-      </c>
       <c r="H10" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="F11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>87</v>
-      </c>
       <c r="H11" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="E12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>92</v>
-      </c>
       <c r="H12" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>99</v>
-      </c>
       <c r="H13" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="G14" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>106</v>
-      </c>
       <c r="H14" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="F15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aakash CLUB REMOVED AS PER PARTH SIR EMAIL
</commit_message>
<xml_diff>
--- a/club.xlsx
+++ b/club.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4518248c6cd0c0d5/Desktop/CSPIT_NEW_2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Websites\CSPIT-NEW-2024\CSPIT_NEW_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{8CB7CD09-CB62-40C2-A613-B48FC6B8C556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A8EE5E1-ABAE-4A9A-AFBC-2B598BD3E184}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="184">
   <si>
     <t>Club ID</t>
   </si>
@@ -360,9 +359,6 @@
   </si>
   <si>
     <t>killolpandya.ec@charusat.ac.in</t>
-  </si>
-  <si>
-    <t>images1\Student Club\ADWITIYA AAKASH - circle - dark.webp</t>
   </si>
   <si>
     <t>images1\Student Club\ML_Club.webp</t>
@@ -666,7 +662,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1051,11 +1047,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1091,13 +1087,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>114</v>
       </c>
       <c r="K1" s="1"/>
     </row>
@@ -1121,48 +1117,48 @@
         <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>119</v>
@@ -1173,20 +1169,17 @@
       <c r="F4" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>120</v>
@@ -1199,15 +1192,15 @@
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:11" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>121</v>
@@ -1215,20 +1208,20 @@
       <c r="E6" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>133</v>
       </c>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>122</v>
@@ -1241,15 +1234,15 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>123</v>
@@ -1257,20 +1250,20 @@
       <c r="E8" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>135</v>
+      <c r="F8" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:11" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>124</v>
@@ -1279,178 +1272,156 @@
         <v>168</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>136</v>
+      <c r="F10" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:11" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>126</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>138</v>
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" ht="345.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>12</v>
+        <v>100</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>128</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="360" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" t="s">
         <v>174</v>
       </c>
       <c r="F15" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="360" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="E16" t="s">
-        <v>175</v>
-      </c>
-      <c r="F16" t="s">
-        <v>142</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" xr:uid="{B3799252-325C-4BA7-83E1-0B4ABA4630D6}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{C053D9B7-E09A-4F85-9B15-3356C9467DDC}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{A130776E-467C-4CF5-A279-81C121EAFA77}"/>
-    <hyperlink ref="C9" r:id="rId4" xr:uid="{C43E63E5-175D-482B-8E60-565A2317DAF1}"/>
-    <hyperlink ref="C8" r:id="rId5" xr:uid="{2EB0C192-8899-4B0D-BC90-80D1B99B5AD3}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{C7E09B01-0EAD-4328-8C47-DBFCB5792DCE}"/>
-    <hyperlink ref="C4" r:id="rId7" xr:uid="{2F6D441B-FE18-407A-A53C-332DADE184B6}"/>
-    <hyperlink ref="C5" r:id="rId8" xr:uid="{D9ABECE2-61DA-4365-A359-C85CF5D16BC9}"/>
-    <hyperlink ref="C6" r:id="rId9" xr:uid="{C9477454-ED77-4337-AC39-DDF8661E5749}"/>
-    <hyperlink ref="C10" r:id="rId10" xr:uid="{C71A858D-5AD9-4C78-8958-2F44E3B2D91B}"/>
-    <hyperlink ref="C11" r:id="rId11" xr:uid="{FA9B5FF1-66E1-4867-BB96-B75C16AF9696}"/>
-    <hyperlink ref="C12" r:id="rId12" xr:uid="{B5F89BDF-DA28-43E9-BC34-ABA3C0433BB1}"/>
-    <hyperlink ref="C13" r:id="rId13" xr:uid="{384BE91D-6FD8-446A-BAA4-C63875390E3C}"/>
-    <hyperlink ref="C14" r:id="rId14" xr:uid="{5F462241-14AD-4645-BE81-22C387C87ACC}"/>
-    <hyperlink ref="C15" r:id="rId15" xr:uid="{25B1CA69-2415-4C8C-AEF6-44FD92D413C8}"/>
-    <hyperlink ref="C16" r:id="rId16" xr:uid="{18DAC898-53DE-4C70-BD52-48C6FF1513F1}"/>
+    <hyperlink ref="H3" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="C8" r:id="rId3"/>
+    <hyperlink ref="C7" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C3" r:id="rId6"/>
+    <hyperlink ref="C4" r:id="rId7"/>
+    <hyperlink ref="C5" r:id="rId8"/>
+    <hyperlink ref="C9" r:id="rId9"/>
+    <hyperlink ref="C10" r:id="rId10"/>
+    <hyperlink ref="C11" r:id="rId11"/>
+    <hyperlink ref="C12" r:id="rId12"/>
+    <hyperlink ref="C13" r:id="rId13"/>
+    <hyperlink ref="C14" r:id="rId14"/>
+    <hyperlink ref="C15" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12E3FC5-108C-49C9-81F8-2E9E0C3472A2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -1467,114 +1438,114 @@
   <sheetData>
     <row r="1" spans="2:6" ht="55.2" x14ac:dyDescent="0.3">
       <c r="B1" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>144</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>147</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="E3" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>150</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="E4" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>153</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="265.2" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>156</v>
-      </c>
       <c r="E5" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="202.8" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D7" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>160</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="B8" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1583,7 +1554,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D451F29C-59FF-4C0E-B76E-5572EE3A7979}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
@@ -1981,7 +1952,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H1" r:id="rId1" xr:uid="{1F77C778-5563-400D-A2FC-3A0BA53796AA}"/>
+    <hyperlink ref="H1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
clubs image issue solved
</commit_message>
<xml_diff>
--- a/club.xlsx
+++ b/club.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="185">
   <si>
     <t>Club ID</t>
   </si>
@@ -562,57 +562,11 @@
     <t>SpiriTech Club</t>
   </si>
   <si>
-    <t>Prof. Harshul Yagnik,faculty coordinator,harshulyagnik.cse@charusat.ac.in,9737642757,CSPIT_Faculty\CSE\HARSHULYAGNIK.webp;Prof. Abhishek Patel,faculty coordinator,abhishekpatel.cse@charusat.ac.in,9099056918,CSPIT_Faculty\CSE\ABHISHEKPATEL.webp</t>
-  </si>
-  <si>
     <t>Prof. Trusha Patel,faculty coordinator,trushagajjar.ce@charusat.ac.in,9624699433,CSPIT_Faculty\CE\TRUSHAPATEL.webp;Prof. Rikita Chokshi,faculty coordinator,rikitachokshi.ce@charusat.ac.in,8780797085,CSPIT_Faculty\CE\RIKITACHOKSHI.webp</t>
-  </si>
-  <si>
-    <t>Dr. Mrugendra Rahevar,faculty coordinator,mrugendrarahevar.ce@charusat.ac.in,9925856399,CSPIT_Faculty\CE\MRUGENDRARAHEVAR.webp;
-Prof. Ronak R Patel,faculty coordinator,ronakrpatel.ce@charusat.ac.in,9409330900,CSPIT_Faculty\CE\RONAKRPATEL.webp;
-Prof. Trusha Patel,faculty coordinator,trushagajjar.ce@charusat.ac.in,9624699443,CSPIT_Faculty\CE\TRUSHAPATEL.webp;
-Prof. Vaishali Koria,faculty coordinator,vaishalimewada.ce@charusat.ac.in,7874114875,CSPIT_Faculty\CE\VAISHALIKORIA.webp</t>
   </si>
   <si>
     <t>Dr. Martin Parmar,faculty coordinator,martinparmar.ce@charusat.ac.in,8238563982,CSPIT_Faculty\CE\MARTINPARMAR.webp;
 Dr. Sneha Padhiar,faculty coordinator,snehapadhiar.ce@charusat.ac.in,9601600000,CSPIT_Faculty\CE\SNEHAPADHIAR.webp</t>
-  </si>
-  <si>
-    <t>Jalpesh Vasa,faculty coordinator,jalpeshvasa.it@charusat.ac.in,9726528769,CSPIT_Faculty\IT\JALPESHVASA.webp;
-Hemant Yadav,faculty coordinator,hemantyadav.it@charusat.ac.in,9327083391,CSPIT_Faculty\IT\HEMANTYADAV.webp</t>
-  </si>
-  <si>
-    <t>Dr. Mrugendra Rahevar,faculty coordinator,mrugendrarahevar.ce@charusat.ac.in,9925856399,CSPIT_Faculty\CE\MRUGENDRARAHEVAR.webp;
-Prof. Ronak N Patel,faculty coordinator,ronakpatel.ce@charusat.ac.in,9913760408,CSPIT_Faculty\CE\RONAKNPATEL.webp;
-Dr. Dhaval Bhoi,faculty coordinator,dhavalbhoi.ce@charusat.ac.in,9879974807,CSPIT_Faculty\CE\DHAVALBHOI.webp</t>
-  </si>
-  <si>
-    <t>Prof. Vikas Panchal,faculty coordinator,vikaspanchal.me@charusat.ac.in,8866286233,CSPIT_Faculty\ME\VIKASPANCHAL.webp;</t>
-  </si>
-  <si>
-    <t>Dr. Arpita Patel,faculty coordinator,N/A,9428661555,CSPIT_Faculty\N/A\ARPITAPATEL.webp</t>
-  </si>
-  <si>
-    <t>Prof. Nishat Shaikh,faculty coordinator,nishatshaikh.it@charusat.ac.in,9979157363,CSPIT_Faculty\IT\NISHATSHAIKH.webp</t>
-  </si>
-  <si>
-    <t>Prof. Nishat Shaikh,faculty coordinator,nishatshaikh.it@charusat.ac.in,9979157363,CSPIT_Faculty\IT\NISHATSHAIKH.webp;
-Dr. Parth Shah,faculty coordinator,parthshah.ce@charusat.ac.in,9925020358,CSPIT_Faculty\CE\PARTHSHAH.webp</t>
-  </si>
-  <si>
-    <t>Prof. Pinal Patel,faculty coordinator,N/A,9979975075,CSPIT_Faculty\N/A\PINALPATEL.webp;
-Prof. Megha Desai,faculty coordinator,N/A,9429032853,CSPIT_Faculty\N/A\MEGHADESAI.webp;
-Prof. Neha Rajput,faculty coordinator,N/A,9099027974,CSPIT_Faculty\N/A\NEHARAJPUT.webp;
-Prof. Gargi Ray,faculty coordinator,N/A,8238042155,CSPIT_Faculty\N/A\GARGIRAY.webp</t>
-  </si>
-  <si>
-    <t>Prof. Kanchal Dave,faculty coordinator,N/A,9973054924,CSPIT_Faculty\N/A\KANCHALDAVE.webp;
-Prof. Mehul Katakiya,faculty coordinator,N/A,8000669363,CSPIT_Faculty\N/A\MEHULKATAKIYA.webp;
-Prof. Vipul Vyas,faculty coordinator,N/A,9727767541,CSPIT_Faculty\N/A\VIPULVYAS.webp;
-Prof. Jay Bhavsar,faculty coordinator,N/A,9898583301,CSPIT_Faculty\N/A\JAYBHAVSAR.webp</t>
-  </si>
-  <si>
-    <t>Dr. Killol Pandya,faculty coordinator,N/A,7600004093,CSPIT_Faculty\N/A\KILLOLPANDYA.webp</t>
   </si>
   <si>
     <t>Dr. Nirav Bhatt,faculty coordinator,niravbhatt.it@charusat.ac.in,9998582812,CSPIT_Faculty\IT\NIRAVBHATT.webp</t>
@@ -657,6 +611,56 @@
 Sanskruti Kukadiya;
 Yug Bhatt;
 Hitarth Khatiwala</t>
+  </si>
+  <si>
+    <t>Prof. Harshul Yagnik,faculty coordinator,harshulyagnik.cse@charusat.ac.in,9737642757,CSPIT_Faculty\CSE\HARSHUL.webp;Prof. Abhishek Patel,faculty coordinator,abhishekpatel.cse@charusat.ac.in,9099056918,CSPIT_Faculty\CSE\ABHISHEK.webp</t>
+  </si>
+  <si>
+    <t>Dr. Martin Parmar,faculty coordinator,martinparmar.ce@charusat.ac.in,8238563982,CSPIT_Faculty\CE\MARTIN.webp;
+Dr. Sneha Padhiar,faculty coordinator,snehapadhiar.ce@charusat.ac.in,9601600000,CSPIT_Faculty\CE\SNEHA.webp</t>
+  </si>
+  <si>
+    <t>Jalpesh Vasa,faculty coordinator,jalpeshvasa.it@charusat.ac.in,9726528769,CSPIT_Faculty\IT\JALPESH.webp;
+Hemant Yadav,faculty coordinator,hemantyadav.it@charusat.ac.in,9327083391,CSPIT_Faculty\IT\HEMANT NANDLALBHAI YADAV.webp</t>
+  </si>
+  <si>
+    <t>Dr. Mrugendra Rahevar,faculty coordinator,MRUGENDRA.ce@charusat.ac.in,9925856399,CSPIT_Faculty\CE\MRUGENDRASINH.webp;
+Prof. Ronak R Patel,faculty coordinator,ronakrpatel.ce@charusat.ac.in,9409330900,CSPIT_Faculty\CE\RONAKKUMAR.webp;
+Prof. Trusha Patel,faculty coordinator,trushagajjar.ce@charusat.ac.in,9624699443,CSPIT_Faculty\CE\TRUSHA.webp;
+Prof. Vaishali Koria,faculty coordinator,vaishalimewada.ce@charusat.ac.in,7874114875,CSPIT_Faculty\CE\VAISHALI.webp</t>
+  </si>
+  <si>
+    <t>Dr. Mrugendra Rahevar,faculty coordinator,MRUGENDRA.ce@charusat.ac.in,9925856399,CSPIT_Faculty\CE\MRUGENDRASINH.webp;
+Prof. Ronak N Patel,faculty coordinator,ronakpatel.ce@charusat.ac.in,9913760408,CSPIT_Faculty\CE\RONAKKUMAR.webp;
+Dr. Dhaval Bhoi,faculty coordinator,dhavalbhoi.ce@charusat.ac.in,9879974807,CSPIT_Faculty\CE\DHAVALKUMAR.webp</t>
+  </si>
+  <si>
+    <t>Prof. Vikas Panchal,faculty coordinator,vikaspanchal.me@charusat.ac.in,8866286233,CSPIT_Faculty\Mechanical\VIKAS.webp;</t>
+  </si>
+  <si>
+    <t>Dr. Arpita Patel,faculty coordinator,arpitapatel.ec@charusat.ac.in,9428661555,CSPIT_Faculty\Electronics\ARPITA.webp</t>
+  </si>
+  <si>
+    <t>Prof. Nishat Shaikh,faculty coordinator,nishatshaikh.it@charusat.ac.in,9979157363,CSPIT_Faculty\IT\NISHAT.webp</t>
+  </si>
+  <si>
+    <t>Prof. Nishat Shaikh,faculty coordinator,nishatshaikh.it@charusat.ac.in,9979157363,CSPIT_Faculty\IT\NISHAT.webp;
+Dr. Parth Shah,faculty coordinator,parthshah.ce@charusat.ac.in,9925020358,CSPIT_Faculty\IT\PARTH.webp</t>
+  </si>
+  <si>
+    <t>Prof. Pinal Patel,faculty coordinator,N/A,9979975075,CSPIT_Faculty\Civil\PINAL.webp;
+Prof. Megha Desai,faculty coordinator,N/A,9429032853,CSPIT_Faculty\Civil\MEGHA.webp;
+Prof. Neha Rajput,faculty coordinator,N/A,9099027974,CSPIT_Faculty\Civil\NEHA.webp;
+Prof. Gargi Ray,faculty coordinator,N/A,8238042155,CSPIT_Faculty\Civil\GARGI.webp</t>
+  </si>
+  <si>
+    <t>Prof. Kanchal Dave,faculty coordinator,N/A,9973054924,CSPIT_Faculty\Civil\KANCHAL.webp;
+Prof. Mehul Katakiya,faculty coordinator,N/A,8000669363,CSPIT_Faculty\Civil\MEHULKUMAR.webp;
+Prof. Vipul Vyas,faculty coordinator,N/A,9727767541,CSPIT_Faculty\Civil\VIPUL.webp;
+Prof. Jay Bhavsar,faculty coordinator,N/A,9898583301,CSPIT_Faculty\Civil\JAY.webp</t>
+  </si>
+  <si>
+    <t>Dr. Killol Pandya,faculty coordinator,N/A,7600004093,CSPIT_Faculty\Electronics\KILLOL.webp</t>
   </si>
 </sst>
 </file>
@@ -1050,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="66" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1140,7 +1144,7 @@
         <v>118</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>130</v>
@@ -1164,14 +1168,14 @@
         <v>119</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>131</v>
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:11" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
@@ -1185,7 +1189,7 @@
         <v>120</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>132</v>
@@ -1206,7 +1210,7 @@
         <v>121</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>133</v>
@@ -1227,7 +1231,7 @@
         <v>122</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>134</v>
@@ -1248,7 +1252,7 @@
         <v>123</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>136</v>
@@ -1269,7 +1273,7 @@
         <v>124</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>135</v>
@@ -1290,7 +1294,7 @@
         <v>125</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>137</v>
@@ -1311,7 +1315,7 @@
         <v>126</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>138</v>
@@ -1332,7 +1336,7 @@
         <v>127</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="F12" s="3"/>
       <c r="H12" s="3"/>
@@ -1351,7 +1355,7 @@
         <v>12</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>139</v>
@@ -1371,7 +1375,7 @@
         <v>128</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="F14" t="s">
         <v>140</v>
@@ -1391,7 +1395,7 @@
         <v>129</v>
       </c>
       <c r="E15" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="F15" t="s">
         <v>141</v>
@@ -1444,7 +1448,7 @@
         <v>143</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>144</v>
@@ -1458,7 +1462,7 @@
         <v>146</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>147</v>
@@ -1472,7 +1476,7 @@
         <v>149</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>150</v>
@@ -1486,7 +1490,7 @@
         <v>152</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>153</v>
@@ -1500,10 +1504,10 @@
         <v>155</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="202.8" x14ac:dyDescent="0.3">
@@ -1514,10 +1518,10 @@
         <v>158</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -1528,7 +1532,7 @@
         <v>159</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>160</v>
@@ -1542,7 +1546,7 @@
         <v>119</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>131</v>

</xml_diff>

<commit_message>
Grow with git club added
</commit_message>
<xml_diff>
--- a/club.xlsx
+++ b/club.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Websites\CSPIT-NEW-2024\CSPIT_NEW_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motat\OneDrive\Desktop\CSPIT_NEW_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6072D9AF-AC14-4573-A75F-478B01942FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="189">
   <si>
     <t>Club ID</t>
   </si>
@@ -53,9 +54,6 @@
   </si>
   <si>
     <t>AWS</t>
-  </si>
-  <si>
-    <t>images1\gallery\AWS Commuinity Day\aws1.webp</t>
   </si>
   <si>
     <t xml:space="preserve">Dulari Bhushan; Parmesh Bhatt </t>
@@ -662,12 +660,29 @@
   <si>
     <t>Dr. Killol Pandya,faculty coordinator,N/A,7600004093,CSPIT_Faculty\Electronics\KILLOL.webp</t>
   </si>
+  <si>
+    <t>GWG</t>
+  </si>
+  <si>
+    <t>Prof. Dhara Solanki,faculty coordinator,dharasolanki.cse@charusat.ac.in,8238448451,CSPIT_Faculty\CSE\DHARA.webp;
+Prof. Srushti Gajjar,faculty coordinator,srushtigajjar.cse@charusat.ac.in,9409546741,CSPIT_Faculty\CSE\SRUSHTI.webp;
+Prof. Brinda Patel,faculty coordinator,brindapatel.cse@charusat.ac.in,7405281125,CSPIT_Faculty\CSE\BRINDA.webp</t>
+  </si>
+  <si>
+    <t>images1\Student Club\git\grow_with_git.png</t>
+  </si>
+  <si>
+    <t>images1\Student Club\git\Github Session.jpg</t>
+  </si>
+  <si>
+    <t>Session on “GITHUB and GITHUB Foundation certification journey under GrowWithGit” Club ; 13 September 2024;A session on GitHub and GitHub Foundation Certification Journey was conducted on 13th September 2024 for the students of the computer science department. The session aimed to introduce the students to the GitHub platform, its certification pathways, and the Microsoft Learn Student Ambassador (MLSA) program. The session was facilitated by Yatharth Chauhan, an esteemed alumnus of the university, who is the founder of Webxela, a GOLD Microsoft Learn Student Ambassador, and a 4X GitHub and LinkedIn certified professional. Yatharth’s extensive experience in these platforms provided valuable insights to the students on how to leverage GitHub certifications for their career growth and development. ;images1\Student Club\git\Github Session.jpg :   images1\Student Club\git\Photo-1.jpg : images1\Student Club\git\Photo-2.png : images1\Student Club\git\Photo-3.png;report1.docx</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -701,6 +716,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -753,23 +774,21 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1051,11 +1070,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="66" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="E16" zoomScale="79" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1064,7 +1083,7 @@
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="21.109375" customWidth="1"/>
     <col min="4" max="4" width="32.88671875" customWidth="1"/>
-    <col min="5" max="5" width="40.77734375" customWidth="1"/>
+    <col min="5" max="5" width="105" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.21875" customWidth="1"/>
     <col min="7" max="7" width="27.88671875" customWidth="1"/>
     <col min="8" max="8" width="47.44140625" customWidth="1"/>
@@ -1091,13 +1110,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>113</v>
       </c>
       <c r="K1" s="1"/>
     </row>
@@ -1109,447 +1128,472 @@
         <v>6</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>17</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G3" s="5"/>
-      <c r="H3" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>21</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>25</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="D7" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:11" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="C8" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>40</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>76</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:11" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>88</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F12" s="3"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>93</v>
-      </c>
       <c r="D13" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>100</v>
-      </c>
       <c r="D14" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="360" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="D15" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E15" t="s">
+        <v>183</v>
+      </c>
+      <c r="F15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="F15" t="s">
-        <v>141</v>
+      <c r="B16" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="C8" r:id="rId3"/>
-    <hyperlink ref="C7" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C3" r:id="rId6"/>
-    <hyperlink ref="C4" r:id="rId7"/>
-    <hyperlink ref="C5" r:id="rId8"/>
-    <hyperlink ref="C9" r:id="rId9"/>
-    <hyperlink ref="C10" r:id="rId10"/>
-    <hyperlink ref="C11" r:id="rId11"/>
-    <hyperlink ref="C12" r:id="rId12"/>
-    <hyperlink ref="C13" r:id="rId13"/>
-    <hyperlink ref="C14" r:id="rId14"/>
-    <hyperlink ref="C15" r:id="rId15"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{D51D8E35-F210-4A14-B90D-208B24FE34DB}"/>
+    <hyperlink ref="G16" r:id="rId16" xr:uid="{8FFF5DCE-5E81-4EA7-B4DE-D42345D92B1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H3" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" style="10"/>
-    <col min="4" max="4" width="100.88671875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="51.44140625" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="10"/>
+    <col min="1" max="3" width="8.88671875" style="3"/>
+    <col min="4" max="4" width="100.88671875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="51.44140625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="E1" s="10" t="s">
+    </row>
+    <row r="2" spans="2:6" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B3" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B3" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="D3" s="15" t="s">
+      <c r="F3" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E3" s="11" t="s">
+    </row>
+    <row r="4" spans="2:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="F4" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E4" s="11" t="s">
+    </row>
+    <row r="5" spans="2:6" ht="265.2" x14ac:dyDescent="0.3">
+      <c r="B5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="265.2" x14ac:dyDescent="0.3">
-      <c r="B5" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D5" s="13" t="s">
+      <c r="F5" s="13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="202.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="D6" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="202.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
+      <c r="F6" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D7" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E7" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D7" s="15" t="s">
+      <c r="F7" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="E7" s="11" t="s">
+    </row>
+    <row r="8" spans="2:6" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="F7" s="15" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>131</v>
+      <c r="F8" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1558,7 +1602,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
@@ -1575,388 +1619,388 @@
         <v>6</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="D3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="H3" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="E4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="H4" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>26</v>
-      </c>
       <c r="E5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="H5" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="E6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="H6" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="E7" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="H7" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="E8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>70</v>
-      </c>
       <c r="H8" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="D9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>73</v>
-      </c>
       <c r="H9" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="H10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>85</v>
-      </c>
       <c r="H11" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>90</v>
-      </c>
       <c r="H12" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>97</v>
-      </c>
       <c r="H13" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="G14" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="H14" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="F15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H1" r:id="rId1"/>
+    <hyperlink ref="H1" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Club details added in excel for first few clubs
</commit_message>
<xml_diff>
--- a/club.xlsx
+++ b/club.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Websites\CSPIT-NEW-2024\CSPIT_NEW_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motat\OneDrive\Desktop\CSPIT_NEW_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353DEABA-C2A5-4D32-BDDF-ECA81A0D980E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="192">
   <si>
     <t>Club ID</t>
   </si>
@@ -368,9 +369,6 @@
   </si>
   <si>
     <t>AWS Cloud Bootcamp;15-17 Nov 2023;A three-day coding event;images1/gallery/AWS Commuinity Day/aws2.webp:images1/gallery/AWS Commuinity Day/aws1.webp:images1/gallery/AWS Commuinity Day/aws3.webp:images1/gallery/AWS Commuinity Day/aws5.webp</t>
-  </si>
-  <si>
-    <t>Certification Bootcamp;2023-10-20;AWS certification bootcamp;bootcamp1.jpg:bootcamp2.jpg;report2.pdf</t>
   </si>
   <si>
     <t>images1/gallery/AWS Commuinity Day/aws2.webp:images1/gallery/AWS Commuinity Day/aws1.webp:images1/gallery/AWS Commuinity Day/aws3.webp:images1/gallery/AWS Commuinity Day/aws5.webp</t>
@@ -449,9 +447,6 @@
 Shrey Lakhtaria</t>
   </si>
   <si>
-    <t>Darshil Chocha; Yupal Chaudhari</t>
-  </si>
-  <si>
     <t>Rinkal Mav</t>
   </si>
   <si>
@@ -555,9 +550,6 @@
     <t>SpiriTech Club</t>
   </si>
   <si>
-    <t>Prof. Trusha Patel,faculty coordinator,trushagajjar.ce@charusat.ac.in,9624699433,CSPIT_Faculty\CE\TRUSHAPATEL.webp;Prof. Rikita Chokshi,faculty coordinator,rikitachokshi.ce@charusat.ac.in,8780797085,CSPIT_Faculty\CE\RIKITACHOKSHI.webp</t>
-  </si>
-  <si>
     <t>Dr. Martin Parmar,faculty coordinator,martinparmar.ce@charusat.ac.in,8238563982,CSPIT_Faculty\CE\MARTINPARMAR.webp;
 Dr. Sneha Padhiar,faculty coordinator,snehapadhiar.ce@charusat.ac.in,9601600000,CSPIT_Faculty\CE\SNEHAPADHIAR.webp</t>
   </si>
@@ -655,11 +647,50 @@
   <si>
     <t>Dr. Killol Pandya,faculty coordinator,N/A,7600004093,CSPIT_Faculty\Electronics\KILLOL.webp</t>
   </si>
+  <si>
+    <t>Apurv Chudasama,22CS016;
+Krushna Parmar ,22AIML028</t>
+  </si>
+  <si>
+    <t>Expert Talk On Introduction to Generative AI with Google Cloud; September 22, 2023.;For students of the CSE department of Computer Science and Engineering, CSPIT, CHARUSAT planned an interactive Expert Talk on Introduction to Generative AI on September 22, 2023. A total of 18 students from Semester 3 participated in the same. When all the students had reported at the CSE AI/ML LAB, we started the workshop at around 2:20 P.M. At the very beginning of the session, students seemed interested to dig deeper into the topic. The expert started the lecture by explaining very basic and real-life examples such as ChatGPT and other AI advancement tools that we use on a daily basis. Thereafter, he continued to explain the same topic on a technical level and how the industry of AI grew and shifted towards it. Furthermore, he gave an idea about how Generative AI is a branch of AI. Compared with the classical machine learning approach, he explained how a machine learning task is different from text/image/music generation. After this, the foundation models were explained which are used to build a Generative AI model. The revolution and LLM, which stands for Large Language Model, were explained thoroughly. To understand the input parameters given to any Generative AI model, prompts are an essential requirement. This topic was explained in depth to help students understand how to generate a prompt to get a perfect output as we want. Different types of prompts were explained nicely (shot prompts). In addition, he explained about the evolution of cloud ML APIs which are providing multipurpose foundation models for AI models, and more concisely explained about Google Cloud and how it can help in the field of Gen AI. Vertex AI was also explained in depth. At the end of this session, the expert provided links and QR codes for GitHub repositories of Generative AI and some other related links to understand Gen AI better and finally concluded with a fruitful discussion and doubt-solving session. ;  images1/Student Club/AIML_CSE/Expert_talk/poster.jpg , images1/Student Club/AIML_CSE/Expert_talk/1.webp , images1/Student Club/AIML_CSE/Expert_talk/2.webp ,  images1/Student Club/AIML_CSE/Expert_talk/3.webp ,  images1/Student Club/AIML_CSE/Expert_talk/4.webp ; images1/Student Club/AIML_CSE/Expert_talk/report.pdf</t>
+  </si>
+  <si>
+    <t>Faculty Workshop on Embedded Machine Learning With NVIDIA Jetson Nano ; 20th June 2023; On 20th June 2023, a one-day hands-on workshop on "Embedded Machine Learning with Nvidia Jetson Nano" was conducted under the Nvidia Academic Hardware Grant Program for the faculty members of CSPIT. A total of 22 faculty members filled out the registration form, and among them, 15 were present for the workshop.
+The workshop aimed to introduce the participants to the fundamentals of embedded machine learning and provide them with practical experience in using the Nvidia Jetson Nano platform for developing machine learning applications. The workshop was led by Prof. Harshul Yagnik from the Department of Computer Science and Engineering, CSPIT.; images1/Student Club/AIML_CSE/faculty_workshop/poster.webp , images1/Student Club/AIML_CSE/faculty_workshop/1.webp , images1/Student Club/AIML_CSE/faculty_workshop/2.webp  ; images1/Student Club/AIML_CSE/faculty_workshop/report.pdf</t>
+  </si>
+  <si>
+    <t>Event 3</t>
+  </si>
+  <si>
+    <t>Peer Learning Session on Nvidia Jetson Nano ; 10 July 2024 ; For the students of 5th sem of the department of CSE, CSPIT the session 1 of the dedicated series on embedded machine learning with Jetson Nano which was focused on Setting up the device and performing classification problems on it was organized by the AI/ML club on 10/07/2024 - Wednesday at Lab 324-D (AIML Department). Total of – 32 students and 4 volunteers attended the workshop. Students reported at the lab at around 12:15 and we started the workshop at 12:20. ; images1/Student Club/AIML_CSE/Peer_learning/poster.webp , images1/Student Club/AIML_CSE/Peer_learning/1.webp , images1/Student Club/AIML_CSE/Peer_learning/2.webp ,  images1/Student Club/AIML_CSE/Peer_learning/3.webp ,  images1/Student Club/AIML_CSE/Peer_learning/4.webp ; images1/Student Club/AIML_CSE/Peer_learning/report.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaushal Bhanderi , 22CE005 ;
+Pooja Ramani , 22CE106 </t>
+  </si>
+  <si>
+    <t>Prof. Trusha Patel,faculty coordinator,trushagajjar.ce@charusat.ac.in,9624699433,CSPIT_Faculty\CE\TRUSHA.webp;Prof. Rikita Chokshi,faculty coordinator,rikitachokshi.ce@charusat.ac.in,8780797085,CSPIT_Faculty\CE\RIKITA.webp</t>
+  </si>
+  <si>
+    <t>Teachers Day Celebration; 5 September 2024; Teachers Day Celeration ;images1/Student Club/TOCC/Teachers_day/poster.webp , images1/Student Club/TOCC/Teachers_day/1.webp , images1/Student Club/TOCC/Teachers_day/2.webp ,  images1/Student Club/TOCC/Teachers_day/3.webp</t>
+  </si>
+  <si>
+    <t>Mehandi Competition ; 19-July 2024 ; Mehandi Competition event provide a wonderful opportunity for students to express their creativity, share their heritage, and learn about the rich cultural backgrounds of their peers.; images1/Student Club/TOCC/MehndiCompetition/poster.webp , images1/Student Club/TOCC/MehndiCompetition/1.webp , images1/Student Club/TOCC/MehndiCompetition/2.webp ,  images1/Student Club/TOCC/MehndiCompetition/3.webp,  images1/Student Club/TOCC/MehndiCompetition/4.webp;images1/Student Club/TOCC/MehndiCompetition/report.pdf</t>
+  </si>
+  <si>
+    <t>CE Department Logo Design Competition; 5 October 2024 ; The workshop titled “CE Department Logo Design Competition” was organized by U.&amp; P U. Patel Department of Computer Engineering. This exciting event was organized mainly aiming for designing a unique and meaningful logo that represents the identity, values, and vision of the CE Department. Participants were encouraged to showcase their creativity, innovation, and design skills by crafting a logo that embodies the spirit of computer engineering and the department's commitment to excellence. ; images1/Student Club/TOCC/logo_competition/poster.webp , images1/Student Club/TOCC/logo_competition/1.webp;  images1/Student Club/TOCC/logo_competition/report.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">images1/Student Club/TOCC/Teachers_day/1.webp : images1/Student Club/TOCC/MehndiCompetition/2.webp : images1/Student Club/TOCC/MehndiCompetition/4.webp : images1/Student Club/TOCC/logo_competition/1.webp </t>
+  </si>
+  <si>
+    <t>Darshil Chocha, 22CE021 ; Yupal Chaudhari , 23CE012</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -717,7 +748,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -726,9 +757,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -743,25 +771,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1044,11 +1063,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="93" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1056,12 +1075,14 @@
     <col min="1" max="1" width="11.21875" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="21.109375" customWidth="1"/>
-    <col min="4" max="4" width="32.88671875" customWidth="1"/>
+    <col min="4" max="4" width="52.109375" customWidth="1"/>
     <col min="5" max="5" width="40.77734375" customWidth="1"/>
     <col min="6" max="6" width="29.21875" customWidth="1"/>
     <col min="7" max="7" width="27.88671875" customWidth="1"/>
     <col min="8" max="8" width="47.44140625" customWidth="1"/>
     <col min="9" max="9" width="31.44140625" customWidth="1"/>
+    <col min="10" max="10" width="26.33203125" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1084,24 +1105,27 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H1" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>112</v>
       </c>
+      <c r="J1" s="7" t="s">
+        <v>183</v>
+      </c>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1114,298 +1138,315 @@
         <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="H2" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+    </row>
+    <row r="3" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="388.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G4" t="s">
+        <v>190</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" ht="302.39999999999998" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="F10" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" ht="345.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" ht="331.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" ht="345.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="F12" s="3"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="F13" s="5" t="s">
+      <c r="E13" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="360" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" t="s">
+        <v>179</v>
+      </c>
+      <c r="F15" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="F14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="360" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E15" t="s">
-        <v>182</v>
-      </c>
-      <c r="F15" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C8" r:id="rId2"/>
-    <hyperlink ref="C7" r:id="rId3"/>
-    <hyperlink ref="C6" r:id="rId4"/>
-    <hyperlink ref="C3" r:id="rId5"/>
-    <hyperlink ref="C4" r:id="rId6"/>
-    <hyperlink ref="C5" r:id="rId7"/>
-    <hyperlink ref="C9" r:id="rId8"/>
-    <hyperlink ref="C10" r:id="rId9"/>
-    <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11"/>
-    <hyperlink ref="C13" r:id="rId12"/>
-    <hyperlink ref="C14" r:id="rId13"/>
-    <hyperlink ref="C15" r:id="rId14"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId15"/>
@@ -1413,7 +1454,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -1422,122 +1463,122 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" style="10"/>
-    <col min="4" max="4" width="100.88671875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="51.44140625" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="10"/>
+    <col min="1" max="3" width="8.88671875" style="3"/>
+    <col min="4" max="4" width="100.88671875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="51.44140625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="13" t="s">
+    </row>
+    <row r="2" spans="2:6" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="D2" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="265.2" x14ac:dyDescent="0.3">
+      <c r="B5" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B3" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="E3" s="11" t="s">
+      <c r="F5" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="202.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="E4" s="11" t="s">
+      <c r="F6" s="11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="265.2" x14ac:dyDescent="0.3">
-      <c r="B5" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="F7" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="202.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>129</v>
+      <c r="F8" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1546,7 +1587,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
@@ -1556,395 +1597,395 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H1" r:id="rId1"/>
+    <hyperlink ref="H1" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Club data added for 22 clubs
</commit_message>
<xml_diff>
--- a/club.xlsx
+++ b/club.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motat\OneDrive\Desktop\CSPIT_NEW_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4518248c6cd0c0d5/Desktop/CSPIT_NEW_2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B4AA31-AE2B-474D-9693-C600DF5AD2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -869,7 +869,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -903,18 +903,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1199,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E15" zoomScale="92" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:I12"/>
+    <sheetView topLeftCell="A24" zoomScale="92" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1557,31 +1545,31 @@
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:13" ht="331.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="3" t="s">
         <v>224</v>
       </c>
       <c r="J11" s="3"/>
@@ -1590,29 +1578,29 @@
       <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:13" ht="216" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14" t="s">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="3" t="s">
         <v>227</v>
       </c>
       <c r="J12" s="3"/>
@@ -1747,8 +1735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1816,7 +1804,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="265.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="109.2" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>147</v>
       </c>
@@ -1830,7 +1818,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="202.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>149</v>
       </c>

</xml_diff>